<commit_message>
updated Gantt, added haversine
</commit_message>
<xml_diff>
--- a/docs/pdfs/Gantt.xlsx
+++ b/docs/pdfs/Gantt.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Task 3</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>Phase 3 Title</t>
   </si>
   <si>
     <t>More Project Management Templates</t>
@@ -252,6 +249,24 @@
   </si>
   <si>
     <t>Data JSON Obect Creation</t>
+  </si>
+  <si>
+    <t>Google Maps Direction Route (Deferred)</t>
+  </si>
+  <si>
+    <t>Distance Calculation (Haversine Formula)</t>
+  </si>
+  <si>
+    <t>Optimizations (Planning in Progress)</t>
+  </si>
+  <si>
+    <t>Adrien</t>
+  </si>
+  <si>
+    <t>Kawai</t>
+  </si>
+  <si>
+    <t>Add DB</t>
   </si>
 </sst>
 </file>
@@ -662,7 +677,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -862,15 +877,9 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,9 +894,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -916,6 +922,13 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -928,13 +941,9 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1200,7 +1209,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1490,7 +1499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1504,8 +1513,8 @@
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1524,10 +1533,10 @@
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1538,25 +1547,25 @@
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="84"/>
+        <v>28</v>
+      </c>
+      <c r="E2" s="81"/>
       <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="94"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="92">
         <f>DATE(2019,10,1)</f>
         <v>43739</v>
@@ -1565,18 +1574,18 @@
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="89">
         <f>I5</f>
-        <v>43738</v>
+        <v>43731</v>
       </c>
       <c r="J4" s="90"/>
       <c r="K4" s="90"/>
@@ -1586,7 +1595,7 @@
       <c r="O4" s="91"/>
       <c r="P4" s="89">
         <f>P5</f>
-        <v>43745</v>
+        <v>43738</v>
       </c>
       <c r="Q4" s="90"/>
       <c r="R4" s="90"/>
@@ -1596,7 +1605,7 @@
       <c r="V4" s="91"/>
       <c r="W4" s="89">
         <f>W5</f>
-        <v>43752</v>
+        <v>43745</v>
       </c>
       <c r="X4" s="90"/>
       <c r="Y4" s="90"/>
@@ -1606,7 +1615,7 @@
       <c r="AC4" s="91"/>
       <c r="AD4" s="89">
         <f>AD5</f>
-        <v>43759</v>
+        <v>43752</v>
       </c>
       <c r="AE4" s="90"/>
       <c r="AF4" s="90"/>
@@ -1616,7 +1625,7 @@
       <c r="AJ4" s="91"/>
       <c r="AK4" s="89">
         <f>AK5</f>
-        <v>43766</v>
+        <v>43759</v>
       </c>
       <c r="AL4" s="90"/>
       <c r="AM4" s="90"/>
@@ -1626,7 +1635,7 @@
       <c r="AQ4" s="91"/>
       <c r="AR4" s="89">
         <f>AR5</f>
-        <v>43773</v>
+        <v>43766</v>
       </c>
       <c r="AS4" s="90"/>
       <c r="AT4" s="90"/>
@@ -1636,7 +1645,7 @@
       <c r="AX4" s="91"/>
       <c r="AY4" s="89">
         <f>AY5</f>
-        <v>43780</v>
+        <v>43773</v>
       </c>
       <c r="AZ4" s="90"/>
       <c r="BA4" s="90"/>
@@ -1646,7 +1655,7 @@
       <c r="BE4" s="91"/>
       <c r="BF4" s="89">
         <f>BF5</f>
-        <v>43787</v>
+        <v>43780</v>
       </c>
       <c r="BG4" s="90"/>
       <c r="BH4" s="90"/>
@@ -1657,242 +1666,242 @@
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
+        <v>41</v>
+      </c>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>43738</v>
+        <v>43731</v>
       </c>
       <c r="J5" s="10">
         <f>I5+1</f>
-        <v>43739</v>
+        <v>43732</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>43740</v>
+        <v>43733</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" si="0"/>
-        <v>43741</v>
+        <v>43734</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>43742</v>
+        <v>43735</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" si="0"/>
-        <v>43743</v>
+        <v>43736</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="0"/>
-        <v>43744</v>
+        <v>43737</v>
       </c>
       <c r="P5" s="11">
         <f>O5+1</f>
-        <v>43745</v>
+        <v>43738</v>
       </c>
       <c r="Q5" s="10">
         <f>P5+1</f>
-        <v>43746</v>
+        <v>43739</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" si="0"/>
-        <v>43747</v>
+        <v>43740</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" si="0"/>
-        <v>43748</v>
+        <v>43741</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" si="0"/>
-        <v>43749</v>
+        <v>43742</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" si="0"/>
-        <v>43750</v>
+        <v>43743</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" si="0"/>
-        <v>43751</v>
+        <v>43744</v>
       </c>
       <c r="W5" s="11">
         <f>V5+1</f>
-        <v>43752</v>
+        <v>43745</v>
       </c>
       <c r="X5" s="10">
         <f>W5+1</f>
-        <v>43753</v>
+        <v>43746</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" si="0"/>
-        <v>43754</v>
+        <v>43747</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" si="0"/>
-        <v>43755</v>
+        <v>43748</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" si="0"/>
-        <v>43756</v>
+        <v>43749</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" si="0"/>
-        <v>43757</v>
+        <v>43750</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="0"/>
-        <v>43758</v>
+        <v>43751</v>
       </c>
       <c r="AD5" s="11">
         <f>AC5+1</f>
-        <v>43759</v>
+        <v>43752</v>
       </c>
       <c r="AE5" s="10">
         <f>AD5+1</f>
-        <v>43760</v>
+        <v>43753</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" si="0"/>
-        <v>43761</v>
+        <v>43754</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" si="0"/>
-        <v>43762</v>
+        <v>43755</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" si="0"/>
-        <v>43763</v>
+        <v>43756</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" si="0"/>
-        <v>43764</v>
+        <v>43757</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" si="0"/>
-        <v>43765</v>
+        <v>43758</v>
       </c>
       <c r="AK5" s="11">
         <f>AJ5+1</f>
-        <v>43766</v>
+        <v>43759</v>
       </c>
       <c r="AL5" s="10">
         <f>AK5+1</f>
-        <v>43767</v>
+        <v>43760</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" si="0"/>
-        <v>43768</v>
+        <v>43761</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" si="0"/>
-        <v>43769</v>
+        <v>43762</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" si="0"/>
-        <v>43770</v>
+        <v>43763</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" si="0"/>
-        <v>43771</v>
+        <v>43764</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" si="0"/>
-        <v>43772</v>
+        <v>43765</v>
       </c>
       <c r="AR5" s="11">
         <f>AQ5+1</f>
-        <v>43773</v>
+        <v>43766</v>
       </c>
       <c r="AS5" s="10">
         <f>AR5+1</f>
-        <v>43774</v>
+        <v>43767</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" si="0"/>
-        <v>43775</v>
+        <v>43768</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" si="0"/>
-        <v>43776</v>
+        <v>43769</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" si="0"/>
-        <v>43777</v>
+        <v>43770</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" si="0"/>
-        <v>43778</v>
+        <v>43771</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" si="0"/>
-        <v>43779</v>
+        <v>43772</v>
       </c>
       <c r="AY5" s="11">
         <f>AX5+1</f>
-        <v>43780</v>
+        <v>43773</v>
       </c>
       <c r="AZ5" s="10">
         <f>AY5+1</f>
-        <v>43781</v>
+        <v>43774</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>43782</v>
+        <v>43775</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" si="1"/>
-        <v>43783</v>
+        <v>43776</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" si="1"/>
-        <v>43784</v>
+        <v>43777</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" si="1"/>
-        <v>43785</v>
+        <v>43778</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" si="1"/>
-        <v>43786</v>
+        <v>43779</v>
       </c>
       <c r="BF5" s="11">
         <f>BE5+1</f>
-        <v>43787</v>
+        <v>43780</v>
       </c>
       <c r="BG5" s="10">
         <f>BF5+1</f>
-        <v>43788</v>
+        <v>43781</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>43789</v>
+        <v>43782</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" si="2"/>
-        <v>43790</v>
+        <v>43783</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" si="2"/>
-        <v>43791</v>
+        <v>43784</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" si="2"/>
-        <v>43792</v>
+        <v>43785</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" si="2"/>
-        <v>43793</v>
+        <v>43786</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
@@ -2140,7 +2149,7 @@
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="62"/>
       <c r="E7"/>
@@ -2207,10 +2216,10 @@
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="70"/>
       <c r="D8" s="19"/>
@@ -2280,13 +2289,13 @@
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="80" t="s">
         <v>49</v>
+      </c>
+      <c r="C9" s="82" t="s">
+        <v>48</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -2363,12 +2372,14 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="83" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="71"/>
+        <v>45</v>
+      </c>
+      <c r="B10" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="82" t="s">
+        <v>48</v>
+      </c>
       <c r="D10" s="22">
         <v>1</v>
       </c>
@@ -2444,10 +2455,12 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
-      <c r="B11" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="71"/>
+      <c r="B11" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="82" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="22">
         <v>1</v>
       </c>
@@ -2523,10 +2536,12 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="58"/>
-      <c r="B12" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="71"/>
+      <c r="B12" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>48</v>
+      </c>
       <c r="D12" s="22">
         <v>1</v>
       </c>
@@ -2602,25 +2617,27 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58"/>
-      <c r="B13" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="71"/>
+      <c r="B13" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>48</v>
+      </c>
       <c r="D13" s="22">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E13" s="66">
         <f>E10+15</f>
         <v>43758</v>
       </c>
       <c r="F13" s="66">
-        <f>E13+3</f>
-        <v>43761</v>
+        <f>E13+5</f>
+        <v>43763</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
@@ -2681,12 +2698,12 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="72"/>
+        <v>55</v>
+      </c>
+      <c r="C14" s="71"/>
       <c r="D14" s="24"/>
       <c r="E14" s="25"/>
       <c r="F14" s="26"/>
@@ -2754,25 +2771,27 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="59"/>
-      <c r="B15" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="73"/>
+      <c r="B15" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="93" t="s">
+        <v>61</v>
+      </c>
       <c r="D15" s="27">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="67">
         <f>E13+6</f>
         <v>43764</v>
       </c>
       <c r="F15" s="67">
-        <f>E15+4</f>
-        <v>43768</v>
+        <f>E15+8</f>
+        <v>43772</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
@@ -2833,25 +2852,27 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="58"/>
-      <c r="B16" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="73"/>
+      <c r="B16" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="93" t="s">
+        <v>62</v>
+      </c>
       <c r="D16" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="E16" s="87">
+        <v>1</v>
+      </c>
+      <c r="E16" s="84">
         <f>E15</f>
         <v>43764</v>
       </c>
-      <c r="F16" s="87">
-        <f>E16+4</f>
-        <v>43768</v>
+      <c r="F16" s="84">
+        <f>E16+18</f>
+        <v>43782</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
@@ -2912,21 +2933,27 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58"/>
-      <c r="B17" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="87" t="s">
-        <v>34</v>
+      <c r="B17" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="E17" s="84">
+        <f>F15+2</f>
+        <v>43774</v>
+      </c>
+      <c r="F17" s="84">
+        <f>E17+4</f>
+        <v>43778</v>
       </c>
       <c r="G17" s="17"/>
-      <c r="H17" s="17" t="e">
+      <c r="H17" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>5</v>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -2987,21 +3014,27 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
-      <c r="B18" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="87" t="s">
-        <v>34</v>
+      <c r="B18" s="83" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="E18" s="84">
+        <f>F17+1</f>
+        <v>43779</v>
+      </c>
+      <c r="F18" s="84">
+        <f>E18+2</f>
+        <v>43781</v>
       </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="17" t="e">
+      <c r="H18" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>3</v>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
@@ -3062,16 +3095,20 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58"/>
-      <c r="B19" s="79" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="87" t="s">
-        <v>34</v>
+      <c r="B19" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0</v>
+      </c>
+      <c r="E19" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="84" t="s">
+        <v>33</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17" t="e">
@@ -3137,12 +3174,12 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="74"/>
+        <v>60</v>
+      </c>
+      <c r="C20" s="72"/>
       <c r="D20" s="29"/>
       <c r="E20" s="30"/>
       <c r="F20" s="31"/>
@@ -3210,16 +3247,16 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="58"/>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="75"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="32"/>
-      <c r="E21" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="88" t="s">
-        <v>34</v>
+      <c r="E21" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="85" t="s">
+        <v>33</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17" t="e">
@@ -3285,16 +3322,16 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="58"/>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="75"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="32"/>
-      <c r="E22" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="88" t="s">
-        <v>34</v>
+      <c r="E22" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="85" t="s">
+        <v>33</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17" t="e">
@@ -3360,16 +3397,16 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58"/>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="75"/>
+      <c r="C23" s="73"/>
       <c r="D23" s="32"/>
-      <c r="E23" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="88" t="s">
-        <v>34</v>
+      <c r="E23" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="85" t="s">
+        <v>33</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17" t="e">
@@ -3435,16 +3472,16 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58"/>
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="75"/>
+      <c r="C24" s="73"/>
       <c r="D24" s="32"/>
-      <c r="E24" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="88" t="s">
-        <v>34</v>
+      <c r="E24" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="85" t="s">
+        <v>33</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17" t="e">
@@ -3510,16 +3547,16 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58"/>
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="75"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="32"/>
-      <c r="E25" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="88" t="s">
-        <v>34</v>
+      <c r="E25" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="85" t="s">
+        <v>33</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17" t="e">
@@ -3585,12 +3622,12 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="76"/>
+        <v>26</v>
+      </c>
+      <c r="C26" s="74"/>
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
       <c r="F26" s="36"/>
@@ -3658,16 +3695,16 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="58"/>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="77"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="37"/>
       <c r="E27" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17" t="e">
@@ -3733,16 +3770,16 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="58"/>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="77"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="37"/>
       <c r="E28" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17" t="e">
@@ -3808,16 +3845,16 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58"/>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="77"/>
+      <c r="C29" s="75"/>
       <c r="D29" s="37"/>
       <c r="E29" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17" t="e">
@@ -3883,16 +3920,16 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="58"/>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="77"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="37"/>
       <c r="E30" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="e">
@@ -3958,16 +3995,16 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="77"/>
+      <c r="C31" s="75"/>
       <c r="D31" s="37"/>
       <c r="E31" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="e">
@@ -4033,10 +4070,10 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="78"/>
+        <v>36</v>
+      </c>
+      <c r="B32" s="79"/>
+      <c r="C32" s="76"/>
       <c r="D32" s="16"/>
       <c r="E32" s="69"/>
       <c r="F32" s="69"/>
@@ -4104,7 +4141,7 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>5</v>
@@ -4187,11 +4224,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4199,6 +4231,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4277,59 +4314,59 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="48" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4339,17 +4376,17 @@
     </row>
     <row r="14" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hand in for nov 15
</commit_message>
<xml_diff>
--- a/docs/pdfs/Gantt.xlsx
+++ b/docs/pdfs/Gantt.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>Task 3</t>
   </si>
@@ -922,6 +922,21 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -929,21 +944,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1209,7 +1209,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1562,118 +1562,118 @@
       <c r="B3" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="92">
+      <c r="D3" s="92"/>
+      <c r="E3" s="90">
         <f>DATE(2019,10,1)</f>
         <v>43739</v>
       </c>
-      <c r="F3" s="92"/>
+      <c r="F3" s="90"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="I4" s="89">
+      <c r="I4" s="87">
         <f>I5</f>
         <v>43731</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="87">
         <f>P5</f>
         <v>43738</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="87">
         <f>W5</f>
         <v>43745</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="87">
         <f>AD5</f>
         <v>43752</v>
       </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="87">
         <f>AK5</f>
         <v>43759</v>
       </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="87">
         <f>AR5</f>
         <v>43766</v>
       </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="89"/>
+      <c r="AY4" s="87">
         <f>AY5</f>
         <v>43773</v>
       </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="89"/>
+      <c r="BF4" s="87">
         <f>BF5</f>
         <v>43780</v>
       </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
+      <c r="BG4" s="88"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="89"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43731</v>
@@ -2774,7 +2774,7 @@
       <c r="B15" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="86" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="27">
@@ -2855,11 +2855,11 @@
       <c r="B16" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="86" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="27">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E16" s="84">
         <f>E15</f>
@@ -2936,7 +2936,7 @@
       <c r="B17" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="86" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="27">
@@ -3017,7 +3017,7 @@
       <c r="B18" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="93" t="s">
+      <c r="C18" s="86" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="27">
@@ -3098,22 +3098,24 @@
       <c r="B19" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="93" t="s">
+      <c r="C19" s="86" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="27">
         <v>0</v>
       </c>
-      <c r="E19" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="84" t="s">
-        <v>33</v>
+      <c r="E19" s="84">
+        <f>F18</f>
+        <v>43781</v>
+      </c>
+      <c r="F19" s="84">
+        <f>E19</f>
+        <v>43781</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="17" t="e">
+      <c r="H19" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
@@ -4224,6 +4226,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4231,11 +4238,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>